<commit_message>
Additional changes in document iaw.  Jira
</commit_message>
<xml_diff>
--- a/Bilder Dokumentation/Arbeitsplanzeitachse und Dokumentation.xlsx
+++ b/Bilder Dokumentation/Arbeitsplanzeitachse und Dokumentation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC32507D-FE4F-41F9-BC31-C0CAD599E5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BAAFFB4-EF0F-4527-8D63-DF8557AA09EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ACC784CE-6BA7-4857-A17F-37B6681AB0C0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>Aktivitäten</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>Optimierung der Website</t>
-  </si>
-  <si>
-    <t>Launch der Website</t>
   </si>
   <si>
     <t>Finales Resümee der Professoren</t>
@@ -1729,7 +1726,7 @@
   <dimension ref="B1:M31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="59" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.69921875" defaultRowHeight="30" customHeight="1"/>
@@ -1839,7 +1836,7 @@
         <v>26</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="2:13" ht="30" customHeight="1">
@@ -1852,7 +1849,7 @@
         <v>24</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>17</v>
@@ -1868,11 +1865,9 @@
         <v>25</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>27</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="G9" s="5"/>
       <c r="M9" t="s">
         <v>20</v>
       </c>
@@ -1885,7 +1880,7 @@
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G10" s="5"/>
     </row>
@@ -2127,35 +2122,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2455,27 +2421,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A03B658-6B9C-459C-845B-B01C985B7A80}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{426B6E75-A903-45DD-90E5-AE11CA3F52A2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70F443D5-8C1F-45A0-9BD5-49725298F08C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2496,6 +2471,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{426B6E75-A903-45DD-90E5-AE11CA3F52A2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A03B658-6B9C-459C-845B-B01C985B7A80}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>

</xml_diff>